<commit_message>
he hecho unas mejoras en el archivo completo con lecturas anuales
</commit_message>
<xml_diff>
--- a/LISTADO_PEDIDO_COMPRAS/data/input/CLASIFICACION_ABC+D_MASCOTAS_VIVO_P1_2025.xlsx
+++ b/LISTADO_PEDIDO_COMPRAS/data/input/CLASIFICACION_ABC+D_MASCOTAS_VIVO_P1_2025.xlsx
@@ -12599,28 +12599,28 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>2707100029</t>
+          <t>2204010007</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>RAMIREZI GOLD</t>
+          <t>CONEJO SUPER TOY PEDIGRI (ORYCTOLAGUS CUNICULUS)</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr"/>
       <c r="D2" s="3" t="inlineStr"/>
       <c r="E2" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2204</t>
         </is>
       </c>
       <c r="F2" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>ANIMAL VIVO PEQUEÑOS MAMIFEROS</t>
         </is>
       </c>
       <c r="G2" s="4" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H2" s="4" t="n">
         <v>0</v>
@@ -12650,10 +12650,10 @@
         <v>59</v>
       </c>
       <c r="Q2" s="4" t="n">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="R2" s="4" t="n">
-        <v>393.33</v>
+        <v>190</v>
       </c>
       <c r="S2" s="5" t="n">
         <v>30</v>
@@ -12665,12 +12665,12 @@
       </c>
       <c r="U2" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 1.59€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V2" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 02/01/2025</t>
         </is>
       </c>
       <c r="W2" s="4" t="inlineStr">
@@ -12682,24 +12682,32 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>2707190007</t>
+          <t>2708010010</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>PANAQUE MAMLUS L104</t>
-        </is>
-      </c>
-      <c r="C3" s="3" t="inlineStr"/>
-      <c r="D3" s="3" t="inlineStr"/>
+          <t>FANTAIL SURTIDO</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>5CM</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>UNICO</t>
+        </is>
+      </c>
       <c r="E3" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2708</t>
         </is>
       </c>
       <c r="F3" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>PECES AGUA FRIA ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G3" s="4" t="n">
@@ -12718,7 +12726,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="4" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="M3" s="5" t="n">
         <v>0</v>
@@ -12727,19 +12735,19 @@
         <v>0</v>
       </c>
       <c r="O3" s="4" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="P3" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q3" s="4" t="n">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="R3" s="4" t="n">
-        <v>393.33</v>
+        <v>53.33</v>
       </c>
       <c r="S3" s="5" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="T3" s="7" t="inlineStr">
         <is>
@@ -12748,12 +12756,12 @@
       </c>
       <c r="U3" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 21.39€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V3" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 20/02/2025</t>
         </is>
       </c>
       <c r="W3" s="4" t="inlineStr">
@@ -12765,24 +12773,24 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>2705040009</t>
+          <t>2707130082</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>HELECHO EN COCO PEQUEÑO</t>
+          <t>RASBORA VERDE NEON</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr"/>
       <c r="D4" s="3" t="inlineStr"/>
       <c r="E4" s="4" t="inlineStr">
         <is>
-          <t>2705</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F4" s="4" t="inlineStr">
         <is>
-          <t>PLANTA ACUATICA DECORACION ACUARIOFILIA</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G4" s="4" t="n">
@@ -12801,7 +12809,7 @@
         <v>0</v>
       </c>
       <c r="L4" s="4" t="n">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="M4" s="5" t="n">
         <v>0</v>
@@ -12810,7 +12818,7 @@
         <v>0</v>
       </c>
       <c r="O4" s="4" t="n">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="P4" s="4" t="n">
         <v>59</v>
@@ -12831,7 +12839,7 @@
       </c>
       <c r="U4" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 6.52€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 43.13€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V4" s="4" t="inlineStr">
@@ -12848,24 +12856,24 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>2708010019</t>
+          <t>2806030007</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>CABEZA DE LEON</t>
+          <t>SHUBUNKIN</t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr"/>
       <c r="D5" s="3" t="inlineStr"/>
       <c r="E5" s="4" t="inlineStr">
         <is>
-          <t>2708</t>
+          <t>2806</t>
         </is>
       </c>
       <c r="F5" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA FRIA ACUARIOFILIA</t>
+          <t>PECES JARDIN ACUATICO</t>
         </is>
       </c>
       <c r="G5" s="4" t="n">
@@ -12884,7 +12892,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="4" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M5" s="5" t="n">
         <v>0</v>
@@ -12893,19 +12901,19 @@
         <v>0</v>
       </c>
       <c r="O5" s="4" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="P5" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q5" s="4" t="n">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="R5" s="4" t="n">
-        <v>126.67</v>
+        <v>393.33</v>
       </c>
       <c r="S5" s="5" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="T5" s="7" t="inlineStr">
         <is>
@@ -12914,12 +12922,12 @@
       </c>
       <c r="U5" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 11.13€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V5" s="4" t="inlineStr">
         <is>
-          <t>Compra 09/02/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W5" s="4" t="inlineStr">
@@ -12931,12 +12939,12 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>2707130021</t>
+          <t>2707120009</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>MELANOTAENIA SURTIDO</t>
+          <t>LORICARIA FILAMENTOSA</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr"/>
@@ -12967,7 +12975,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="4" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="M6" s="5" t="n">
         <v>0</v>
@@ -12976,19 +12984,19 @@
         <v>0</v>
       </c>
       <c r="O6" s="4" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="P6" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q6" s="4" t="n">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="R6" s="4" t="n">
-        <v>126.67</v>
+        <v>393.33</v>
       </c>
       <c r="S6" s="5" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="T6" s="7" t="inlineStr">
         <is>
@@ -12997,12 +13005,12 @@
       </c>
       <c r="U6" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 19.74€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V6" s="4" t="inlineStr">
         <is>
-          <t>Compra 09/02/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W6" s="4" t="inlineStr">
@@ -13014,24 +13022,24 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>2705040011</t>
+          <t>2707100013</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>BAMBU CUEVA</t>
+          <t>NANACARA ANOMALA</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr"/>
       <c r="D7" s="3" t="inlineStr"/>
       <c r="E7" s="4" t="inlineStr">
         <is>
-          <t>2705</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F7" s="4" t="inlineStr">
         <is>
-          <t>PLANTA ACUATICA DECORACION ACUARIOFILIA</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G7" s="4" t="n">
@@ -13050,7 +13058,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M7" s="5" t="n">
         <v>0</v>
@@ -13059,19 +13067,19 @@
         <v>0</v>
       </c>
       <c r="O7" s="4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="P7" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q7" s="4" t="n">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="R7" s="4" t="n">
-        <v>393.33</v>
+        <v>126.67</v>
       </c>
       <c r="S7" s="5" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="T7" s="7" t="inlineStr">
         <is>
@@ -13080,12 +13088,12 @@
       </c>
       <c r="U7" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 14.32€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V7" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 09/02/2025</t>
         </is>
       </c>
       <c r="W7" s="4" t="inlineStr">
@@ -13097,24 +13105,24 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>2707100024</t>
+          <t>2708020003</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>APISTOGRAMA BORELLI</t>
+          <t>ORANDA SURTIDO</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr"/>
       <c r="D8" s="3" t="inlineStr"/>
       <c r="E8" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2708</t>
         </is>
       </c>
       <c r="F8" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>PECES AGUA FRIA ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G8" s="4" t="n">
@@ -13133,7 +13141,7 @@
         <v>0</v>
       </c>
       <c r="L8" s="4" t="n">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="M8" s="5" t="n">
         <v>0</v>
@@ -13142,16 +13150,16 @@
         <v>0</v>
       </c>
       <c r="O8" s="4" t="n">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="P8" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q8" s="4" t="n">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="R8" s="4" t="n">
-        <v>313.33</v>
+        <v>393.33</v>
       </c>
       <c r="S8" s="5" t="n">
         <v>30</v>
@@ -13163,12 +13171,12 @@
       </c>
       <c r="U8" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 59.5€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V8" s="4" t="inlineStr">
         <is>
-          <t>Compra 12/01/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W8" s="4" t="inlineStr">
@@ -13180,12 +13188,12 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>2707070003</t>
+          <t>2707130031</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>TETRA PRISTELLA ROJA INIRIDA</t>
+          <t>PEZ DOLAR PLATA</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr"/>
@@ -13216,7 +13224,7 @@
         <v>0</v>
       </c>
       <c r="L9" s="4" t="n">
-        <v>105</v>
+        <v>2</v>
       </c>
       <c r="M9" s="5" t="n">
         <v>0</v>
@@ -13225,7 +13233,7 @@
         <v>0</v>
       </c>
       <c r="O9" s="4" t="n">
-        <v>105</v>
+        <v>2</v>
       </c>
       <c r="P9" s="4" t="n">
         <v>59</v>
@@ -13246,7 +13254,7 @@
       </c>
       <c r="U9" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 44.1€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 3.35€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V9" s="4" t="inlineStr">
@@ -13263,24 +13271,32 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>2707130020</t>
+          <t>2708010014</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>LABEO ZORRO VOLADOR</t>
-        </is>
-      </c>
-      <c r="C10" s="3" t="inlineStr"/>
-      <c r="D10" s="3" t="inlineStr"/>
+          <t>RYUKIN SURTIDO</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>5I6</t>
+        </is>
+      </c>
+      <c r="D10" s="3" t="inlineStr">
+        <is>
+          <t>UNICO</t>
+        </is>
+      </c>
       <c r="E10" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2708</t>
         </is>
       </c>
       <c r="F10" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>PECES AGUA FRIA ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G10" s="4" t="n">
@@ -13299,7 +13315,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="4" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="M10" s="5" t="n">
         <v>0</v>
@@ -13308,16 +13324,16 @@
         <v>0</v>
       </c>
       <c r="O10" s="4" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="P10" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q10" s="4" t="n">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="R10" s="4" t="n">
-        <v>393.33</v>
+        <v>380</v>
       </c>
       <c r="S10" s="5" t="n">
         <v>30</v>
@@ -13329,12 +13345,12 @@
       </c>
       <c r="U10" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 8.32€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V10" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 02/01/2025</t>
         </is>
       </c>
       <c r="W10" s="4" t="inlineStr">
@@ -13346,24 +13362,24 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>2707130018</t>
+          <t>2705040003</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>GARRA RUFA ARCOIRIS FLAVATRA</t>
+          <t>PLANTA ACUATICA XL</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr"/>
       <c r="D11" s="3" t="inlineStr"/>
       <c r="E11" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2705</t>
         </is>
       </c>
       <c r="F11" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>PLANTA ACUATICA DECORACION ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G11" s="4" t="n">
@@ -13382,7 +13398,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="4" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="M11" s="5" t="n">
         <v>0</v>
@@ -13391,7 +13407,7 @@
         <v>0</v>
       </c>
       <c r="O11" s="4" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="P11" s="4" t="n">
         <v>59</v>
@@ -13412,7 +13428,7 @@
       </c>
       <c r="U11" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 7.56€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 14.29€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V11" s="4" t="inlineStr">
@@ -13429,12 +13445,12 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>2707130083</t>
+          <t>2707100040</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>POPONDETA PASKAI</t>
+          <t>RAMIREZI BOLIVIANO (PAPILIOCHROMIS ALTISPINOSA)</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr"/>
@@ -13480,10 +13496,10 @@
         <v>59</v>
       </c>
       <c r="Q12" s="4" t="n">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="R12" s="4" t="n">
-        <v>313.33</v>
+        <v>220</v>
       </c>
       <c r="S12" s="5" t="n">
         <v>30</v>
@@ -13500,7 +13516,7 @@
       </c>
       <c r="V12" s="4" t="inlineStr">
         <is>
-          <t>Compra 12/01/2025</t>
+          <t>Compra 26/01/2025</t>
         </is>
       </c>
       <c r="W12" s="4" t="inlineStr">
@@ -13512,12 +13528,12 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>2707080006</t>
+          <t>2707050026</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>ESCALAR RED DEVIL</t>
+          <t>BETTA MACHO LONG TAIL</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr"/>
@@ -13548,7 +13564,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="4" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="M13" s="5" t="n">
         <v>0</v>
@@ -13557,19 +13573,19 @@
         <v>0</v>
       </c>
       <c r="O13" s="4" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="P13" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q13" s="4" t="n">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="R13" s="4" t="n">
-        <v>33.33</v>
+        <v>393.33</v>
       </c>
       <c r="S13" s="5" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="T13" s="7" t="inlineStr">
         <is>
@@ -13578,12 +13594,12 @@
       </c>
       <c r="U13" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.92€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V13" s="4" t="inlineStr">
         <is>
-          <t>Compra 23/02/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W13" s="4" t="inlineStr">
@@ -13595,12 +13611,12 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>2707050026</t>
+          <t>2707130026</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>BETTA MACHO LONG TAIL</t>
+          <t>PANGASIUS SUTCHI</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr"/>
@@ -13631,7 +13647,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="4" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M14" s="5" t="n">
         <v>0</v>
@@ -13640,7 +13656,7 @@
         <v>0</v>
       </c>
       <c r="O14" s="4" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="P14" s="4" t="n">
         <v>59</v>
@@ -13661,7 +13677,7 @@
       </c>
       <c r="U14" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.92€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 15.15€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V14" s="4" t="inlineStr">
@@ -13678,32 +13694,24 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>2708010014</t>
+          <t>2705040006</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>RYUKIN SURTIDO</t>
-        </is>
-      </c>
-      <c r="C15" s="3" t="inlineStr">
-        <is>
-          <t>5I6</t>
-        </is>
-      </c>
-      <c r="D15" s="3" t="inlineStr">
-        <is>
-          <t>UNICO</t>
-        </is>
-      </c>
+          <t>ANUBIA MIX COCO HALF</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="inlineStr"/>
+      <c r="D15" s="3" t="inlineStr"/>
       <c r="E15" s="4" t="inlineStr">
         <is>
-          <t>2708</t>
+          <t>2705</t>
         </is>
       </c>
       <c r="F15" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA FRIA ACUARIOFILIA</t>
+          <t>PLANTA ACUATICA DECORACION ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G15" s="4" t="n">
@@ -13722,7 +13730,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="4" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="M15" s="5" t="n">
         <v>0</v>
@@ -13731,16 +13739,16 @@
         <v>0</v>
       </c>
       <c r="O15" s="4" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="P15" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q15" s="4" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="R15" s="4" t="n">
-        <v>380</v>
+        <v>393.33</v>
       </c>
       <c r="S15" s="5" t="n">
         <v>30</v>
@@ -13752,12 +13760,12 @@
       </c>
       <c r="U15" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 57.24€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V15" s="4" t="inlineStr">
         <is>
-          <t>Compra 02/01/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W15" s="4" t="inlineStr">
@@ -13769,12 +13777,12 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>2707130031</t>
+          <t>2707100024</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>PEZ DOLAR PLATA</t>
+          <t>APISTOGRAMA BORELLI</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr"/>
@@ -13820,10 +13828,10 @@
         <v>59</v>
       </c>
       <c r="Q16" s="4" t="n">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="R16" s="4" t="n">
-        <v>393.33</v>
+        <v>313.33</v>
       </c>
       <c r="S16" s="5" t="n">
         <v>30</v>
@@ -13835,12 +13843,12 @@
       </c>
       <c r="U16" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 3.35€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V16" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 12/01/2025</t>
         </is>
       </c>
       <c r="W16" s="4" t="inlineStr">
@@ -13852,28 +13860,28 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>2606050000</t>
+          <t>2707130035</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>BICHO PALO</t>
+          <t>PEZ HACHA</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr"/>
       <c r="D17" s="3" t="inlineStr"/>
       <c r="E17" s="4" t="inlineStr">
         <is>
-          <t>2606</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F17" s="4" t="inlineStr">
         <is>
-          <t>ANIMAL VIVO REPTILES</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G17" s="4" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H17" s="4" t="n">
         <v>0</v>
@@ -13888,7 +13896,7 @@
         <v>0</v>
       </c>
       <c r="L17" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M17" s="5" t="n">
         <v>0</v>
@@ -13897,19 +13905,19 @@
         <v>0</v>
       </c>
       <c r="O17" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P17" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q17" s="4" t="n">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="R17" s="4" t="n">
-        <v>63.33</v>
+        <v>393.33</v>
       </c>
       <c r="S17" s="5" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="T17" s="7" t="inlineStr">
         <is>
@@ -13918,12 +13926,12 @@
       </c>
       <c r="U17" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 1.18€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V17" s="4" t="inlineStr">
         <is>
-          <t>Compra 09/02/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W17" s="4" t="inlineStr">
@@ -13935,12 +13943,12 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>2707130075</t>
+          <t>2707170002</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>PEZ MEDIO PICO BUFON (HEMIRHAMPHODON KUEKENTHALI)</t>
+          <t>PEZ SIERRA SELECTO</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr"/>
@@ -13971,7 +13979,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M18" s="5" t="n">
         <v>0</v>
@@ -13980,7 +13988,7 @@
         <v>0</v>
       </c>
       <c r="O18" s="4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P18" s="4" t="n">
         <v>59</v>
@@ -14001,7 +14009,7 @@
       </c>
       <c r="U18" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 4.26€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 7.15€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V18" s="4" t="inlineStr">
@@ -14018,24 +14026,24 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>2707130084</t>
+          <t>2708010007</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>PANCHAX RAYADO</t>
+          <t>COMETA SARASA</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr"/>
       <c r="D19" s="3" t="inlineStr"/>
       <c r="E19" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2708</t>
         </is>
       </c>
       <c r="F19" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>PECES AGUA FRIA ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G19" s="4" t="n">
@@ -14054,7 +14062,7 @@
         <v>0</v>
       </c>
       <c r="L19" s="4" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M19" s="5" t="n">
         <v>0</v>
@@ -14063,19 +14071,19 @@
         <v>0</v>
       </c>
       <c r="O19" s="4" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="P19" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q19" s="4" t="n">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="R19" s="4" t="n">
-        <v>33.33</v>
+        <v>393.33</v>
       </c>
       <c r="S19" s="5" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="T19" s="7" t="inlineStr">
         <is>
@@ -14084,12 +14092,12 @@
       </c>
       <c r="U19" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 7.84€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V19" s="4" t="inlineStr">
         <is>
-          <t>Compra 23/02/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W19" s="4" t="inlineStr">
@@ -14101,24 +14109,24 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>2707100013</t>
+          <t>2705040010</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>NANACARA ANOMALA</t>
+          <t>BAMBU PIRAMIDE</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr"/>
       <c r="D20" s="3" t="inlineStr"/>
       <c r="E20" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2705</t>
         </is>
       </c>
       <c r="F20" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>PLANTA ACUATICA DECORACION ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G20" s="4" t="n">
@@ -14137,7 +14145,7 @@
         <v>0</v>
       </c>
       <c r="L20" s="4" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M20" s="5" t="n">
         <v>0</v>
@@ -14146,19 +14154,19 @@
         <v>0</v>
       </c>
       <c r="O20" s="4" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="P20" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q20" s="4" t="n">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="R20" s="4" t="n">
-        <v>126.67</v>
+        <v>393.33</v>
       </c>
       <c r="S20" s="5" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="T20" s="7" t="inlineStr">
         <is>
@@ -14167,12 +14175,12 @@
       </c>
       <c r="U20" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 20.98€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V20" s="4" t="inlineStr">
         <is>
-          <t>Compra 09/02/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W20" s="4" t="inlineStr">
@@ -14184,28 +14192,28 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>2104090002</t>
+          <t>2707190007</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>DIAMANTE BICHENOW (POEPHILA BICHENOVII) DIABI</t>
+          <t>PANAQUE MAMLUS L104</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr"/>
       <c r="D21" s="3" t="inlineStr"/>
       <c r="E21" s="4" t="inlineStr">
         <is>
-          <t>2104</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F21" s="4" t="inlineStr">
         <is>
-          <t>ANIMAL VIVO PAJARO</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G21" s="4" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H21" s="4" t="n">
         <v>0</v>
@@ -14220,7 +14228,7 @@
         <v>0</v>
       </c>
       <c r="L21" s="4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M21" s="5" t="n">
         <v>0</v>
@@ -14229,7 +14237,7 @@
         <v>0</v>
       </c>
       <c r="O21" s="4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P21" s="4" t="n">
         <v>59</v>
@@ -14238,7 +14246,7 @@
         <v>59</v>
       </c>
       <c r="R21" s="4" t="n">
-        <v>196.67</v>
+        <v>393.33</v>
       </c>
       <c r="S21" s="5" t="n">
         <v>30</v>
@@ -14250,7 +14258,7 @@
       </c>
       <c r="U21" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 15.4€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 21.39€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V21" s="4" t="inlineStr">
@@ -14267,24 +14275,24 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>2707170006</t>
+          <t>2708010019</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
         <is>
-          <t>BADIS ESCARLATA</t>
+          <t>CABEZA DE LEON</t>
         </is>
       </c>
       <c r="C22" s="3" t="inlineStr"/>
       <c r="D22" s="3" t="inlineStr"/>
       <c r="E22" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2708</t>
         </is>
       </c>
       <c r="F22" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>PECES AGUA FRIA ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G22" s="4" t="n">
@@ -14303,7 +14311,7 @@
         <v>0</v>
       </c>
       <c r="L22" s="4" t="n">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="M22" s="5" t="n">
         <v>0</v>
@@ -14312,19 +14320,19 @@
         <v>0</v>
       </c>
       <c r="O22" s="4" t="n">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="P22" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q22" s="4" t="n">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="R22" s="4" t="n">
-        <v>393.33</v>
+        <v>126.67</v>
       </c>
       <c r="S22" s="5" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="T22" s="7" t="inlineStr">
         <is>
@@ -14333,12 +14341,12 @@
       </c>
       <c r="U22" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 20.48€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V22" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 09/02/2025</t>
         </is>
       </c>
       <c r="W22" s="4" t="inlineStr">
@@ -14350,12 +14358,12 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>2707130035</t>
+          <t>2707100028</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>PEZ HACHA</t>
+          <t>PARACHROMIS MOTAGUENSIS 8-11 (CICLIDO JAGUAR ROJO)</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr"/>
@@ -14416,7 +14424,7 @@
       </c>
       <c r="U23" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 1.18€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 3.57€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V23" s="4" t="inlineStr">
@@ -14433,28 +14441,28 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>2708010007</t>
+          <t>2104090002</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
         <is>
-          <t>COMETA SARASA</t>
+          <t>DIAMANTE BICHENOW (POEPHILA BICHENOVII) DIABI</t>
         </is>
       </c>
       <c r="C24" s="3" t="inlineStr"/>
       <c r="D24" s="3" t="inlineStr"/>
       <c r="E24" s="4" t="inlineStr">
         <is>
-          <t>2708</t>
+          <t>2104</t>
         </is>
       </c>
       <c r="F24" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA FRIA ACUARIOFILIA</t>
+          <t>ANIMAL VIVO PAJARO</t>
         </is>
       </c>
       <c r="G24" s="4" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H24" s="4" t="n">
         <v>0</v>
@@ -14469,7 +14477,7 @@
         <v>0</v>
       </c>
       <c r="L24" s="4" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="M24" s="5" t="n">
         <v>0</v>
@@ -14478,7 +14486,7 @@
         <v>0</v>
       </c>
       <c r="O24" s="4" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="P24" s="4" t="n">
         <v>59</v>
@@ -14487,7 +14495,7 @@
         <v>59</v>
       </c>
       <c r="R24" s="4" t="n">
-        <v>393.33</v>
+        <v>196.67</v>
       </c>
       <c r="S24" s="5" t="n">
         <v>30</v>
@@ -14499,7 +14507,7 @@
       </c>
       <c r="U24" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 7.84€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 15.4€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V24" s="4" t="inlineStr">
@@ -14516,12 +14524,12 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>2707040007</t>
+          <t>2707130083</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>BARBO SAWBWA</t>
+          <t>POPONDETA PASKAI</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr"/>
@@ -14552,7 +14560,7 @@
         <v>0</v>
       </c>
       <c r="L25" s="4" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="M25" s="5" t="n">
         <v>0</v>
@@ -14561,19 +14569,19 @@
         <v>0</v>
       </c>
       <c r="O25" s="4" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="P25" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q25" s="4" t="n">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="R25" s="4" t="n">
-        <v>33.33</v>
+        <v>313.33</v>
       </c>
       <c r="S25" s="5" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="T25" s="7" t="inlineStr">
         <is>
@@ -14582,12 +14590,12 @@
       </c>
       <c r="U25" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V25" s="4" t="inlineStr">
         <is>
-          <t>Compra 23/02/2025</t>
+          <t>Compra 12/01/2025</t>
         </is>
       </c>
       <c r="W25" s="4" t="inlineStr">
@@ -14599,24 +14607,24 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>2606010004</t>
+          <t>2104090006</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
         <is>
-          <t>TORTUGA RUSA (AGRIONEMYS HORSFIELDII)</t>
+          <t>FORPUS MUTACION AZUL (FORPUS COELESTIS)</t>
         </is>
       </c>
       <c r="C26" s="3" t="inlineStr"/>
       <c r="D26" s="3" t="inlineStr"/>
       <c r="E26" s="4" t="inlineStr">
         <is>
-          <t>2606</t>
+          <t>2104</t>
         </is>
       </c>
       <c r="F26" s="4" t="inlineStr">
         <is>
-          <t>ANIMAL VIVO REPTILES</t>
+          <t>ANIMAL VIVO PAJARO</t>
         </is>
       </c>
       <c r="G26" s="4" t="n">
@@ -14635,7 +14643,7 @@
         <v>0</v>
       </c>
       <c r="L26" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M26" s="5" t="n">
         <v>0</v>
@@ -14644,7 +14652,7 @@
         <v>0</v>
       </c>
       <c r="O26" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P26" s="4" t="n">
         <v>59</v>
@@ -14665,7 +14673,7 @@
       </c>
       <c r="U26" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 43.83€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 49.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V26" s="4" t="inlineStr">
@@ -14682,12 +14690,12 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>2707130047</t>
+          <t>2707070003</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
         <is>
-          <t>RASBORA MACULATUS</t>
+          <t>TETRA PRISTELLA ROJA INIRIDA</t>
         </is>
       </c>
       <c r="C27" s="3" t="inlineStr"/>
@@ -14718,7 +14726,7 @@
         <v>0</v>
       </c>
       <c r="L27" s="4" t="n">
-        <v>27</v>
+        <v>105</v>
       </c>
       <c r="M27" s="5" t="n">
         <v>0</v>
@@ -14727,7 +14735,7 @@
         <v>0</v>
       </c>
       <c r="O27" s="4" t="n">
-        <v>27</v>
+        <v>105</v>
       </c>
       <c r="P27" s="4" t="n">
         <v>59</v>
@@ -14748,7 +14756,7 @@
       </c>
       <c r="U27" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 15.31€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 44.1€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V27" s="4" t="inlineStr">
@@ -14765,12 +14773,12 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>2707110022</t>
+          <t>2707110005</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
         <is>
-          <t>CORYDORA ORANGE VENEZUELA</t>
+          <t>BOTIA MORLETI 4</t>
         </is>
       </c>
       <c r="C28" s="3" t="inlineStr"/>
@@ -14801,7 +14809,7 @@
         <v>0</v>
       </c>
       <c r="L28" s="4" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="M28" s="5" t="n">
         <v>0</v>
@@ -14810,7 +14818,7 @@
         <v>0</v>
       </c>
       <c r="O28" s="4" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="P28" s="4" t="n">
         <v>59</v>
@@ -14831,7 +14839,7 @@
       </c>
       <c r="U28" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 9.58€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 2.31€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V28" s="4" t="inlineStr">
@@ -14848,12 +14856,12 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>2707100038</t>
+          <t>2707130018</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
         <is>
-          <t>RAMIREZI BLACK DEVIL</t>
+          <t>GARRA RUFA ARCOIRIS FLAVATRA</t>
         </is>
       </c>
       <c r="C29" s="3" t="inlineStr"/>
@@ -14884,7 +14892,7 @@
         <v>0</v>
       </c>
       <c r="L29" s="4" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="M29" s="5" t="n">
         <v>0</v>
@@ -14893,7 +14901,7 @@
         <v>0</v>
       </c>
       <c r="O29" s="4" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="P29" s="4" t="n">
         <v>59</v>
@@ -14914,7 +14922,7 @@
       </c>
       <c r="U29" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 28.48€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 7.56€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V29" s="4" t="inlineStr">
@@ -14931,24 +14939,24 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>2708010014</t>
+          <t>2707120001</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
         <is>
-          <t>RYUKIN SURTIDO</t>
+          <t>HYPANCISTRUS SP L333 5-6</t>
         </is>
       </c>
       <c r="C30" s="3" t="inlineStr"/>
       <c r="D30" s="3" t="inlineStr"/>
       <c r="E30" s="4" t="inlineStr">
         <is>
-          <t>2708</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F30" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA FRIA ACUARIOFILIA</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G30" s="4" t="n">
@@ -14967,7 +14975,7 @@
         <v>0</v>
       </c>
       <c r="L30" s="4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="M30" s="5" t="n">
         <v>0</v>
@@ -14976,7 +14984,7 @@
         <v>0</v>
       </c>
       <c r="O30" s="4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="P30" s="4" t="n">
         <v>59</v>
@@ -14997,7 +15005,7 @@
       </c>
       <c r="U30" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 31.5€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 10.64€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V30" s="4" t="inlineStr">
@@ -15014,32 +15022,24 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>2708010010</t>
+          <t>2707130006</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
         <is>
-          <t>FANTAIL SURTIDO</t>
-        </is>
-      </c>
-      <c r="C31" s="3" t="inlineStr">
-        <is>
-          <t>5CM</t>
-        </is>
-      </c>
-      <c r="D31" s="3" t="inlineStr">
-        <is>
-          <t>UNICO</t>
-        </is>
-      </c>
+          <t>CRISTAL DE JAVA - BICHIRRI CRISTAL</t>
+        </is>
+      </c>
+      <c r="C31" s="3" t="inlineStr"/>
+      <c r="D31" s="3" t="inlineStr"/>
       <c r="E31" s="4" t="inlineStr">
         <is>
-          <t>2708</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F31" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA FRIA ACUARIOFILIA</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G31" s="4" t="n">
@@ -15058,7 +15058,7 @@
         <v>0</v>
       </c>
       <c r="L31" s="4" t="n">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="M31" s="5" t="n">
         <v>0</v>
@@ -15067,19 +15067,19 @@
         <v>0</v>
       </c>
       <c r="O31" s="4" t="n">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="P31" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q31" s="4" t="n">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="R31" s="4" t="n">
-        <v>53.33</v>
+        <v>393.33</v>
       </c>
       <c r="S31" s="5" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="T31" s="7" t="inlineStr">
         <is>
@@ -15088,12 +15088,12 @@
       </c>
       <c r="U31" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 5.33€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V31" s="4" t="inlineStr">
         <is>
-          <t>Compra 20/02/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W31" s="4" t="inlineStr">
@@ -15105,24 +15105,24 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>2705040010</t>
+          <t>2708010014</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
         <is>
-          <t>BAMBU PIRAMIDE</t>
+          <t>RYUKIN SURTIDO</t>
         </is>
       </c>
       <c r="C32" s="3" t="inlineStr"/>
       <c r="D32" s="3" t="inlineStr"/>
       <c r="E32" s="4" t="inlineStr">
         <is>
-          <t>2705</t>
+          <t>2708</t>
         </is>
       </c>
       <c r="F32" s="4" t="inlineStr">
         <is>
-          <t>PLANTA ACUATICA DECORACION ACUARIOFILIA</t>
+          <t>PECES AGUA FRIA ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G32" s="4" t="n">
@@ -15141,7 +15141,7 @@
         <v>0</v>
       </c>
       <c r="L32" s="4" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="M32" s="5" t="n">
         <v>0</v>
@@ -15150,7 +15150,7 @@
         <v>0</v>
       </c>
       <c r="O32" s="4" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="P32" s="4" t="n">
         <v>59</v>
@@ -15171,7 +15171,7 @@
       </c>
       <c r="U32" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 20.98€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 31.5€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V32" s="4" t="inlineStr">
@@ -15188,28 +15188,28 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>2707100028</t>
+          <t>2104090001</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
         <is>
-          <t>PARACHROMIS MOTAGUENSIS 8-11 (CICLIDO JAGUAR ROJO)</t>
+          <t>DIAMANTE BARBERO COLA LARGA</t>
         </is>
       </c>
       <c r="C33" s="3" t="inlineStr"/>
       <c r="D33" s="3" t="inlineStr"/>
       <c r="E33" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2104</t>
         </is>
       </c>
       <c r="F33" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>ANIMAL VIVO PAJARO</t>
         </is>
       </c>
       <c r="G33" s="4" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H33" s="4" t="n">
         <v>0</v>
@@ -15242,7 +15242,7 @@
         <v>59</v>
       </c>
       <c r="R33" s="4" t="n">
-        <v>393.33</v>
+        <v>196.67</v>
       </c>
       <c r="S33" s="5" t="n">
         <v>30</v>
@@ -15254,7 +15254,7 @@
       </c>
       <c r="U33" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 3.57€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 15.4€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V33" s="4" t="inlineStr">
@@ -15271,12 +15271,12 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>2707100004</t>
+          <t>2707130020</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
         <is>
-          <t>APISTOGRAMA CACATUOIDES</t>
+          <t>LABEO ZORRO VOLADOR</t>
         </is>
       </c>
       <c r="C34" s="3" t="inlineStr"/>
@@ -15307,7 +15307,7 @@
         <v>0</v>
       </c>
       <c r="L34" s="4" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="M34" s="5" t="n">
         <v>0</v>
@@ -15316,7 +15316,7 @@
         <v>0</v>
       </c>
       <c r="O34" s="4" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="P34" s="4" t="n">
         <v>59</v>
@@ -15337,7 +15337,7 @@
       </c>
       <c r="U34" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 2.79€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 8.32€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V34" s="4" t="inlineStr">
@@ -15354,12 +15354,12 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>2707040006</t>
+          <t>2707090002</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
         <is>
-          <t>BARBO ARCOIRIS (NOTROPIS CHROSOMUS)</t>
+          <t>CICLIDO TANGANICA SURTIDO</t>
         </is>
       </c>
       <c r="C35" s="3" t="inlineStr"/>
@@ -15390,7 +15390,7 @@
         <v>0</v>
       </c>
       <c r="L35" s="4" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="M35" s="5" t="n">
         <v>0</v>
@@ -15399,19 +15399,19 @@
         <v>0</v>
       </c>
       <c r="O35" s="4" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="P35" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q35" s="4" t="n">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="R35" s="4" t="n">
-        <v>33.33</v>
+        <v>393.33</v>
       </c>
       <c r="S35" s="5" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="T35" s="7" t="inlineStr">
         <is>
@@ -15420,12 +15420,12 @@
       </c>
       <c r="U35" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 4.9€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V35" s="4" t="inlineStr">
         <is>
-          <t>Compra 23/02/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W35" s="4" t="inlineStr">
@@ -15437,28 +15437,28 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>2104080001</t>
+          <t>2707120003</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
         <is>
-          <t>PERIQUITO BURQUE</t>
+          <t>LORICARIA SP RED</t>
         </is>
       </c>
       <c r="C36" s="3" t="inlineStr"/>
       <c r="D36" s="3" t="inlineStr"/>
       <c r="E36" s="4" t="inlineStr">
         <is>
-          <t>2104</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F36" s="4" t="inlineStr">
         <is>
-          <t>ANIMAL VIVO PAJARO</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G36" s="4" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H36" s="4" t="n">
         <v>0</v>
@@ -15473,7 +15473,7 @@
         <v>0</v>
       </c>
       <c r="L36" s="4" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M36" s="5" t="n">
         <v>0</v>
@@ -15482,7 +15482,7 @@
         <v>0</v>
       </c>
       <c r="O36" s="4" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P36" s="4" t="n">
         <v>59</v>
@@ -15491,7 +15491,7 @@
         <v>59</v>
       </c>
       <c r="R36" s="4" t="n">
-        <v>196.67</v>
+        <v>393.33</v>
       </c>
       <c r="S36" s="5" t="n">
         <v>30</v>
@@ -15503,7 +15503,7 @@
       </c>
       <c r="U36" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 24.5€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 11.3€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V36" s="4" t="inlineStr">
@@ -15520,28 +15520,28 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>2104090006</t>
+          <t>2707130075</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
         <is>
-          <t>FORPUS MUTACION AZUL (FORPUS COELESTIS)</t>
+          <t>PEZ MEDIO PICO BUFON (HEMIRHAMPHODON KUEKENTHALI)</t>
         </is>
       </c>
       <c r="C37" s="3" t="inlineStr"/>
       <c r="D37" s="3" t="inlineStr"/>
       <c r="E37" s="4" t="inlineStr">
         <is>
-          <t>2104</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F37" s="4" t="inlineStr">
         <is>
-          <t>ANIMAL VIVO PAJARO</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G37" s="4" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H37" s="4" t="n">
         <v>0</v>
@@ -15556,7 +15556,7 @@
         <v>0</v>
       </c>
       <c r="L37" s="4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M37" s="5" t="n">
         <v>0</v>
@@ -15565,7 +15565,7 @@
         <v>0</v>
       </c>
       <c r="O37" s="4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P37" s="4" t="n">
         <v>59</v>
@@ -15574,7 +15574,7 @@
         <v>59</v>
       </c>
       <c r="R37" s="4" t="n">
-        <v>196.67</v>
+        <v>393.33</v>
       </c>
       <c r="S37" s="5" t="n">
         <v>30</v>
@@ -15586,7 +15586,7 @@
       </c>
       <c r="U37" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 49.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 4.26€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V37" s="4" t="inlineStr">
@@ -15603,12 +15603,12 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>2707120003</t>
+          <t>2707130084</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
         <is>
-          <t>LORICARIA SP RED</t>
+          <t>PANCHAX RAYADO</t>
         </is>
       </c>
       <c r="C38" s="3" t="inlineStr"/>
@@ -15639,7 +15639,7 @@
         <v>0</v>
       </c>
       <c r="L38" s="4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M38" s="5" t="n">
         <v>0</v>
@@ -15648,19 +15648,19 @@
         <v>0</v>
       </c>
       <c r="O38" s="4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P38" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q38" s="4" t="n">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="R38" s="4" t="n">
-        <v>393.33</v>
+        <v>33.33</v>
       </c>
       <c r="S38" s="5" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="T38" s="7" t="inlineStr">
         <is>
@@ -15669,12 +15669,12 @@
       </c>
       <c r="U38" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 11.3€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V38" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 23/02/2025</t>
         </is>
       </c>
       <c r="W38" s="4" t="inlineStr">
@@ -15686,16 +15686,24 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>2705040003</t>
+          <t>2705040004</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
         <is>
-          <t>PLANTA ACUATICA XL</t>
-        </is>
-      </c>
-      <c r="C39" s="3" t="inlineStr"/>
-      <c r="D39" s="3" t="inlineStr"/>
+          <t>PLANTAS EN TRONCO</t>
+        </is>
+      </c>
+      <c r="C39" s="3" t="inlineStr">
+        <is>
+          <t>3UD</t>
+        </is>
+      </c>
+      <c r="D39" s="3" t="inlineStr">
+        <is>
+          <t>UNICO</t>
+        </is>
+      </c>
       <c r="E39" s="4" t="inlineStr">
         <is>
           <t>2705</t>
@@ -15722,7 +15730,7 @@
         <v>0</v>
       </c>
       <c r="L39" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M39" s="5" t="n">
         <v>0</v>
@@ -15731,7 +15739,7 @@
         <v>0</v>
       </c>
       <c r="O39" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P39" s="4" t="n">
         <v>59</v>
@@ -15752,7 +15760,7 @@
       </c>
       <c r="U39" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 14.29€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 12.35€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V39" s="4" t="inlineStr">
@@ -15769,12 +15777,12 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>2707120007</t>
+          <t>2707170006</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
         <is>
-          <t>PANAQUE REAL L190</t>
+          <t>BADIS ESCARLATA</t>
         </is>
       </c>
       <c r="C40" s="3" t="inlineStr"/>
@@ -15805,7 +15813,7 @@
         <v>0</v>
       </c>
       <c r="L40" s="4" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="M40" s="5" t="n">
         <v>0</v>
@@ -15814,7 +15822,7 @@
         <v>0</v>
       </c>
       <c r="O40" s="4" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="P40" s="4" t="n">
         <v>59</v>
@@ -15835,7 +15843,7 @@
       </c>
       <c r="U40" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 10.72€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 20.48€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V40" s="4" t="inlineStr">
@@ -15852,24 +15860,16 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>2707110006</t>
+          <t>2707090010</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
         <is>
-          <t>BOTIA PAYASO</t>
-        </is>
-      </c>
-      <c r="C41" s="3" t="inlineStr">
-        <is>
-          <t>7CM</t>
-        </is>
-      </c>
-      <c r="D41" s="3" t="inlineStr">
-        <is>
-          <t>UNICO</t>
-        </is>
-      </c>
+          <t>KANDANGO ROJO</t>
+        </is>
+      </c>
+      <c r="C41" s="3" t="inlineStr"/>
+      <c r="D41" s="3" t="inlineStr"/>
       <c r="E41" s="4" t="inlineStr">
         <is>
           <t>2707</t>
@@ -15926,7 +15926,7 @@
       </c>
       <c r="U41" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 5.91€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 6.29€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V41" s="4" t="inlineStr">
@@ -15943,12 +15943,12 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>2707120001</t>
+          <t>2707100004</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
         <is>
-          <t>HYPANCISTRUS SP L333 5-6</t>
+          <t>APISTOGRAMA CACATUOIDES</t>
         </is>
       </c>
       <c r="C42" s="3" t="inlineStr"/>
@@ -15979,7 +15979,7 @@
         <v>0</v>
       </c>
       <c r="L42" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M42" s="5" t="n">
         <v>0</v>
@@ -15988,7 +15988,7 @@
         <v>0</v>
       </c>
       <c r="O42" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P42" s="4" t="n">
         <v>59</v>
@@ -16009,7 +16009,7 @@
       </c>
       <c r="U42" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 10.64€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 2.79€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V42" s="4" t="inlineStr">
@@ -16026,12 +16026,12 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>2707110005</t>
+          <t>2707100038</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
         <is>
-          <t>BOTIA MORLETI 4</t>
+          <t>RAMIREZI BLACK DEVIL</t>
         </is>
       </c>
       <c r="C43" s="3" t="inlineStr"/>
@@ -16062,7 +16062,7 @@
         <v>0</v>
       </c>
       <c r="L43" s="4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M43" s="5" t="n">
         <v>0</v>
@@ -16071,7 +16071,7 @@
         <v>0</v>
       </c>
       <c r="O43" s="4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="P43" s="4" t="n">
         <v>59</v>
@@ -16092,7 +16092,7 @@
       </c>
       <c r="U43" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 2.31€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 28.48€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V43" s="4" t="inlineStr">
@@ -16109,24 +16109,16 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>2707130025</t>
+          <t>2707040006</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
         <is>
-          <t>PANGASIUS ALBINO</t>
-        </is>
-      </c>
-      <c r="C44" s="3" t="inlineStr">
-        <is>
-          <t>6I7</t>
-        </is>
-      </c>
-      <c r="D44" s="3" t="inlineStr">
-        <is>
-          <t>UNICO</t>
-        </is>
-      </c>
+          <t>BARBO ARCOIRIS (NOTROPIS CHROSOMUS)</t>
+        </is>
+      </c>
+      <c r="C44" s="3" t="inlineStr"/>
+      <c r="D44" s="3" t="inlineStr"/>
       <c r="E44" s="4" t="inlineStr">
         <is>
           <t>2707</t>
@@ -16153,7 +16145,7 @@
         <v>0</v>
       </c>
       <c r="L44" s="4" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="M44" s="5" t="n">
         <v>0</v>
@@ -16162,19 +16154,19 @@
         <v>0</v>
       </c>
       <c r="O44" s="4" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="P44" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q44" s="4" t="n">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="R44" s="4" t="n">
-        <v>393.33</v>
+        <v>33.33</v>
       </c>
       <c r="S44" s="5" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="T44" s="7" t="inlineStr">
         <is>
@@ -16183,12 +16175,12 @@
       </c>
       <c r="U44" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 5.1€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V44" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 23/02/2025</t>
         </is>
       </c>
       <c r="W44" s="4" t="inlineStr">
@@ -16200,24 +16192,24 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>2707130054</t>
+          <t>2705040011</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
         <is>
-          <t>PEZ CUCHILLO PAYASO</t>
+          <t>BAMBU CUEVA</t>
         </is>
       </c>
       <c r="C45" s="3" t="inlineStr"/>
       <c r="D45" s="3" t="inlineStr"/>
       <c r="E45" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2705</t>
         </is>
       </c>
       <c r="F45" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>PLANTA ACUATICA DECORACION ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G45" s="4" t="n">
@@ -16236,7 +16228,7 @@
         <v>0</v>
       </c>
       <c r="L45" s="4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M45" s="5" t="n">
         <v>0</v>
@@ -16245,7 +16237,7 @@
         <v>0</v>
       </c>
       <c r="O45" s="4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P45" s="4" t="n">
         <v>59</v>
@@ -16266,7 +16258,7 @@
       </c>
       <c r="U45" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 3.09€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 14.32€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V45" s="4" t="inlineStr">
@@ -16283,28 +16275,28 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>2705040008</t>
+          <t>2606010004</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
         <is>
-          <t>ANUBIA EN ROCA</t>
+          <t>TORTUGA RUSA (AGRIONEMYS HORSFIELDII)</t>
         </is>
       </c>
       <c r="C46" s="3" t="inlineStr"/>
       <c r="D46" s="3" t="inlineStr"/>
       <c r="E46" s="4" t="inlineStr">
         <is>
-          <t>2705</t>
+          <t>2606</t>
         </is>
       </c>
       <c r="F46" s="4" t="inlineStr">
         <is>
-          <t>PLANTA ACUATICA DECORACION ACUARIOFILIA</t>
+          <t>ANIMAL VIVO REPTILES</t>
         </is>
       </c>
       <c r="G46" s="4" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H46" s="4" t="n">
         <v>0</v>
@@ -16319,7 +16311,7 @@
         <v>0</v>
       </c>
       <c r="L46" s="4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M46" s="5" t="n">
         <v>0</v>
@@ -16328,7 +16320,7 @@
         <v>0</v>
       </c>
       <c r="O46" s="4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P46" s="4" t="n">
         <v>59</v>
@@ -16337,7 +16329,7 @@
         <v>59</v>
       </c>
       <c r="R46" s="4" t="n">
-        <v>393.33</v>
+        <v>196.67</v>
       </c>
       <c r="S46" s="5" t="n">
         <v>30</v>
@@ -16349,7 +16341,7 @@
       </c>
       <c r="U46" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 10.27€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 43.83€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V46" s="4" t="inlineStr">
@@ -16366,28 +16358,28 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>2104080003</t>
+          <t>2707090009</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
         <is>
-          <t>PERIQUITO INGLES (MELOPSITTACUS UNDULATUS)</t>
+          <t>AULONOCARA CALICO RED NEON</t>
         </is>
       </c>
       <c r="C47" s="3" t="inlineStr"/>
       <c r="D47" s="3" t="inlineStr"/>
       <c r="E47" s="4" t="inlineStr">
         <is>
-          <t>2104</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F47" s="4" t="inlineStr">
         <is>
-          <t>ANIMAL VIVO PAJARO</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G47" s="4" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H47" s="4" t="n">
         <v>0</v>
@@ -16402,7 +16394,7 @@
         <v>0</v>
       </c>
       <c r="L47" s="4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M47" s="5" t="n">
         <v>0</v>
@@ -16411,7 +16403,7 @@
         <v>0</v>
       </c>
       <c r="O47" s="4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P47" s="4" t="n">
         <v>59</v>
@@ -16420,7 +16412,7 @@
         <v>59</v>
       </c>
       <c r="R47" s="4" t="n">
-        <v>196.67</v>
+        <v>393.33</v>
       </c>
       <c r="S47" s="5" t="n">
         <v>30</v>
@@ -16432,7 +16424,7 @@
       </c>
       <c r="U47" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 67.2€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 7.31€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V47" s="4" t="inlineStr">
@@ -16449,16 +16441,24 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>2707050001</t>
+          <t>2707130025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
         <is>
-          <t>BESUCON HELOSTOMA TEMMINCKII</t>
-        </is>
-      </c>
-      <c r="C48" s="3" t="inlineStr"/>
-      <c r="D48" s="3" t="inlineStr"/>
+          <t>PANGASIUS ALBINO</t>
+        </is>
+      </c>
+      <c r="C48" s="3" t="inlineStr">
+        <is>
+          <t>6I7</t>
+        </is>
+      </c>
+      <c r="D48" s="3" t="inlineStr">
+        <is>
+          <t>UNICO</t>
+        </is>
+      </c>
       <c r="E48" s="4" t="inlineStr">
         <is>
           <t>2707</t>
@@ -16485,7 +16485,7 @@
         <v>0</v>
       </c>
       <c r="L48" s="4" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M48" s="5" t="n">
         <v>0</v>
@@ -16494,19 +16494,19 @@
         <v>0</v>
       </c>
       <c r="O48" s="4" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P48" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q48" s="4" t="n">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="R48" s="4" t="n">
-        <v>33.33</v>
+        <v>393.33</v>
       </c>
       <c r="S48" s="5" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="T48" s="7" t="inlineStr">
         <is>
@@ -16515,12 +16515,12 @@
       </c>
       <c r="U48" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 5.1€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V48" s="4" t="inlineStr">
         <is>
-          <t>Compra 23/02/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W48" s="4" t="inlineStr">
@@ -16532,24 +16532,24 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>2707110001</t>
+          <t>2705040008</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
         <is>
-          <t>BOTIA CARA CABALLO</t>
+          <t>ANUBIA EN ROCA</t>
         </is>
       </c>
       <c r="C49" s="3" t="inlineStr"/>
       <c r="D49" s="3" t="inlineStr"/>
       <c r="E49" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2705</t>
         </is>
       </c>
       <c r="F49" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>PLANTA ACUATICA DECORACION ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G49" s="4" t="n">
@@ -16568,7 +16568,7 @@
         <v>0</v>
       </c>
       <c r="L49" s="4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M49" s="5" t="n">
         <v>0</v>
@@ -16577,7 +16577,7 @@
         <v>0</v>
       </c>
       <c r="O49" s="4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P49" s="4" t="n">
         <v>59</v>
@@ -16598,7 +16598,7 @@
       </c>
       <c r="U49" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 3.54€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 10.27€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V49" s="4" t="inlineStr">
@@ -16615,12 +16615,12 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>2707050022</t>
+          <t>2707110001</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
         <is>
-          <t>BETTA KOI</t>
+          <t>BOTIA CARA CABALLO</t>
         </is>
       </c>
       <c r="C50" s="3" t="inlineStr"/>
@@ -16651,7 +16651,7 @@
         <v>0</v>
       </c>
       <c r="L50" s="4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M50" s="5" t="n">
         <v>0</v>
@@ -16660,19 +16660,19 @@
         <v>0</v>
       </c>
       <c r="O50" s="4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P50" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q50" s="4" t="n">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="R50" s="4" t="n">
-        <v>126.67</v>
+        <v>393.33</v>
       </c>
       <c r="S50" s="5" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="T50" s="7" t="inlineStr">
         <is>
@@ -16681,12 +16681,12 @@
       </c>
       <c r="U50" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 3.54€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V50" s="4" t="inlineStr">
         <is>
-          <t>Compra 09/02/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W50" s="4" t="inlineStr">
@@ -16698,24 +16698,24 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>2705040006</t>
+          <t>2707050001</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
         <is>
-          <t>ANUBIA MIX COCO HALF</t>
+          <t>BESUCON HELOSTOMA TEMMINCKII</t>
         </is>
       </c>
       <c r="C51" s="3" t="inlineStr"/>
       <c r="D51" s="3" t="inlineStr"/>
       <c r="E51" s="4" t="inlineStr">
         <is>
-          <t>2705</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F51" s="4" t="inlineStr">
         <is>
-          <t>PLANTA ACUATICA DECORACION ACUARIOFILIA</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G51" s="4" t="n">
@@ -16734,7 +16734,7 @@
         <v>0</v>
       </c>
       <c r="L51" s="4" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="M51" s="5" t="n">
         <v>0</v>
@@ -16743,19 +16743,19 @@
         <v>0</v>
       </c>
       <c r="O51" s="4" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="P51" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q51" s="4" t="n">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="R51" s="4" t="n">
-        <v>393.33</v>
+        <v>33.33</v>
       </c>
       <c r="S51" s="5" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="T51" s="7" t="inlineStr">
         <is>
@@ -16764,12 +16764,12 @@
       </c>
       <c r="U51" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 57.24€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V51" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 23/02/2025</t>
         </is>
       </c>
       <c r="W51" s="4" t="inlineStr">
@@ -16781,12 +16781,12 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>2707110023</t>
+          <t>2707100002</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
         <is>
-          <t>BOTIA SUMO</t>
+          <t>ANDINOACARA PULCHER AZUL ELECTRICO 3-4</t>
         </is>
       </c>
       <c r="C52" s="3" t="inlineStr"/>
@@ -16817,7 +16817,7 @@
         <v>0</v>
       </c>
       <c r="L52" s="4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M52" s="5" t="n">
         <v>0</v>
@@ -16826,7 +16826,7 @@
         <v>0</v>
       </c>
       <c r="O52" s="4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="P52" s="4" t="n">
         <v>59</v>
@@ -16847,7 +16847,7 @@
       </c>
       <c r="U52" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 11.13€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 1.47€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V52" s="4" t="inlineStr">
@@ -16864,24 +16864,24 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>2806030007</t>
+          <t>2707100016</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
         <is>
-          <t>SHUBUNKIN</t>
+          <t>RAMIREZI ALEMAN AZUL (MIKROGEOPHAGUS)</t>
         </is>
       </c>
       <c r="C53" s="3" t="inlineStr"/>
       <c r="D53" s="3" t="inlineStr"/>
       <c r="E53" s="4" t="inlineStr">
         <is>
-          <t>2806</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F53" s="4" t="inlineStr">
         <is>
-          <t>PECES JARDIN ACUATICO</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G53" s="4" t="n">
@@ -16900,7 +16900,7 @@
         <v>0</v>
       </c>
       <c r="L53" s="4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M53" s="5" t="n">
         <v>0</v>
@@ -16909,16 +16909,16 @@
         <v>0</v>
       </c>
       <c r="O53" s="4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P53" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q53" s="4" t="n">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="R53" s="4" t="n">
-        <v>393.33</v>
+        <v>220</v>
       </c>
       <c r="S53" s="5" t="n">
         <v>30</v>
@@ -16930,12 +16930,12 @@
       </c>
       <c r="U53" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 11.13€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V53" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 26/01/2025</t>
         </is>
       </c>
       <c r="W53" s="4" t="inlineStr">
@@ -16947,12 +16947,12 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>2707130006</t>
+          <t>2707130047</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
         <is>
-          <t>CRISTAL DE JAVA - BICHIRRI CRISTAL</t>
+          <t>RASBORA MACULATUS</t>
         </is>
       </c>
       <c r="C54" s="3" t="inlineStr"/>
@@ -16983,7 +16983,7 @@
         <v>0</v>
       </c>
       <c r="L54" s="4" t="n">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="M54" s="5" t="n">
         <v>0</v>
@@ -16992,7 +16992,7 @@
         <v>0</v>
       </c>
       <c r="O54" s="4" t="n">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="P54" s="4" t="n">
         <v>59</v>
@@ -17013,7 +17013,7 @@
       </c>
       <c r="U54" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 5.33€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 15.31€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V54" s="4" t="inlineStr">
@@ -17030,28 +17030,28 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>2707100016</t>
+          <t>2805040003</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
         <is>
-          <t>RAMIREZI ALEMAN AZUL (MIKROGEOPHAGUS)</t>
+          <t>PLANTA FLOTANTE MINI</t>
         </is>
       </c>
       <c r="C55" s="3" t="inlineStr"/>
       <c r="D55" s="3" t="inlineStr"/>
       <c r="E55" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2805</t>
         </is>
       </c>
       <c r="F55" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>PLANTAS JARDIN ACUATICO</t>
         </is>
       </c>
       <c r="G55" s="4" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H55" s="4" t="n">
         <v>0</v>
@@ -17066,7 +17066,7 @@
         <v>0</v>
       </c>
       <c r="L55" s="4" t="n">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="M55" s="5" t="n">
         <v>0</v>
@@ -17075,16 +17075,16 @@
         <v>0</v>
       </c>
       <c r="O55" s="4" t="n">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="P55" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q55" s="4" t="n">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="R55" s="4" t="n">
-        <v>220</v>
+        <v>173.33</v>
       </c>
       <c r="S55" s="5" t="n">
         <v>30</v>
@@ -17101,7 +17101,7 @@
       </c>
       <c r="V55" s="4" t="inlineStr">
         <is>
-          <t>Compra 26/01/2025</t>
+          <t>Compra 07/01/2025</t>
         </is>
       </c>
       <c r="W55" s="4" t="inlineStr">
@@ -17113,12 +17113,12 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>2707090009</t>
+          <t>2707050028</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
         <is>
-          <t>AULONOCARA CALICO RED NEON</t>
+          <t>BETTA HELLBOY MACHO</t>
         </is>
       </c>
       <c r="C56" s="3" t="inlineStr"/>
@@ -17149,7 +17149,7 @@
         <v>0</v>
       </c>
       <c r="L56" s="4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M56" s="5" t="n">
         <v>0</v>
@@ -17158,19 +17158,19 @@
         <v>0</v>
       </c>
       <c r="O56" s="4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P56" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q56" s="4" t="n">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="R56" s="4" t="n">
-        <v>393.33</v>
+        <v>33.33</v>
       </c>
       <c r="S56" s="5" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="T56" s="7" t="inlineStr">
         <is>
@@ -17179,12 +17179,12 @@
       </c>
       <c r="U56" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 7.31€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V56" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 23/02/2025</t>
         </is>
       </c>
       <c r="W56" s="4" t="inlineStr">
@@ -17196,12 +17196,12 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>2707130026</t>
+          <t>2707050019</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
         <is>
-          <t>PANGASIUS SUTCHI</t>
+          <t>PEZ PARAISO MACROPODUS</t>
         </is>
       </c>
       <c r="C57" s="3" t="inlineStr"/>
@@ -17262,7 +17262,7 @@
       </c>
       <c r="U57" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 15.15€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 1.96€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V57" s="4" t="inlineStr">
@@ -17279,28 +17279,28 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>2806030001</t>
+          <t>2104080003</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
         <is>
-          <t>COMETA SURTIDO XXL</t>
+          <t>PERIQUITO INGLES (MELOPSITTACUS UNDULATUS)</t>
         </is>
       </c>
       <c r="C58" s="3" t="inlineStr"/>
       <c r="D58" s="3" t="inlineStr"/>
       <c r="E58" s="4" t="inlineStr">
         <is>
-          <t>2806</t>
+          <t>2104</t>
         </is>
       </c>
       <c r="F58" s="4" t="inlineStr">
         <is>
-          <t>PECES JARDIN ACUATICO</t>
+          <t>ANIMAL VIVO PAJARO</t>
         </is>
       </c>
       <c r="G58" s="4" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H58" s="4" t="n">
         <v>0</v>
@@ -17315,7 +17315,7 @@
         <v>0</v>
       </c>
       <c r="L58" s="4" t="n">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="M58" s="5" t="n">
         <v>0</v>
@@ -17324,7 +17324,7 @@
         <v>0</v>
       </c>
       <c r="O58" s="4" t="n">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="P58" s="4" t="n">
         <v>59</v>
@@ -17333,7 +17333,7 @@
         <v>59</v>
       </c>
       <c r="R58" s="4" t="n">
-        <v>393.33</v>
+        <v>196.67</v>
       </c>
       <c r="S58" s="5" t="n">
         <v>30</v>
@@ -17345,7 +17345,7 @@
       </c>
       <c r="U58" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 51.56€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 67.2€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V58" s="4" t="inlineStr">
@@ -17362,12 +17362,12 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>2707100011</t>
+          <t>2707100029</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
         <is>
-          <t>HEROS SEVERUM</t>
+          <t>RAMIREZI GOLD</t>
         </is>
       </c>
       <c r="C59" s="3" t="inlineStr"/>
@@ -17398,7 +17398,7 @@
         <v>0</v>
       </c>
       <c r="L59" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M59" s="5" t="n">
         <v>0</v>
@@ -17407,16 +17407,16 @@
         <v>0</v>
       </c>
       <c r="O59" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P59" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q59" s="4" t="n">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="R59" s="4" t="n">
-        <v>313.33</v>
+        <v>393.33</v>
       </c>
       <c r="S59" s="5" t="n">
         <v>30</v>
@@ -17428,12 +17428,12 @@
       </c>
       <c r="U59" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 1.59€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V59" s="4" t="inlineStr">
         <is>
-          <t>Compra 12/01/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W59" s="4" t="inlineStr">
@@ -17445,24 +17445,24 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>2708020003</t>
+          <t>2806030001</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
         <is>
-          <t>ORANDA SURTIDO</t>
+          <t>COMETA SURTIDO XXL</t>
         </is>
       </c>
       <c r="C60" s="3" t="inlineStr"/>
       <c r="D60" s="3" t="inlineStr"/>
       <c r="E60" s="4" t="inlineStr">
         <is>
-          <t>2708</t>
+          <t>2806</t>
         </is>
       </c>
       <c r="F60" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA FRIA ACUARIOFILIA</t>
+          <t>PECES JARDIN ACUATICO</t>
         </is>
       </c>
       <c r="G60" s="4" t="n">
@@ -17481,7 +17481,7 @@
         <v>0</v>
       </c>
       <c r="L60" s="4" t="n">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="M60" s="5" t="n">
         <v>0</v>
@@ -17490,7 +17490,7 @@
         <v>0</v>
       </c>
       <c r="O60" s="4" t="n">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="P60" s="4" t="n">
         <v>59</v>
@@ -17511,7 +17511,7 @@
       </c>
       <c r="U60" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 59.5€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 51.56€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V60" s="4" t="inlineStr">
@@ -17528,12 +17528,12 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>2707050019</t>
+          <t>2707080006</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
         <is>
-          <t>PEZ PARAISO MACROPODUS</t>
+          <t>ESCALAR RED DEVIL</t>
         </is>
       </c>
       <c r="C61" s="3" t="inlineStr"/>
@@ -17564,7 +17564,7 @@
         <v>0</v>
       </c>
       <c r="L61" s="4" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="M61" s="5" t="n">
         <v>0</v>
@@ -17573,19 +17573,19 @@
         <v>0</v>
       </c>
       <c r="O61" s="4" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="P61" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q61" s="4" t="n">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="R61" s="4" t="n">
-        <v>393.33</v>
+        <v>33.33</v>
       </c>
       <c r="S61" s="5" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="T61" s="7" t="inlineStr">
         <is>
@@ -17594,12 +17594,12 @@
       </c>
       <c r="U61" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 1.96€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V61" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 23/02/2025</t>
         </is>
       </c>
       <c r="W61" s="4" t="inlineStr">
@@ -17611,28 +17611,28 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>2104090001</t>
+          <t>2707100011</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
         <is>
-          <t>DIAMANTE BARBERO COLA LARGA</t>
+          <t>HEROS SEVERUM</t>
         </is>
       </c>
       <c r="C62" s="3" t="inlineStr"/>
       <c r="D62" s="3" t="inlineStr"/>
       <c r="E62" s="4" t="inlineStr">
         <is>
-          <t>2104</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F62" s="4" t="inlineStr">
         <is>
-          <t>ANIMAL VIVO PAJARO</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G62" s="4" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H62" s="4" t="n">
         <v>0</v>
@@ -17647,7 +17647,7 @@
         <v>0</v>
       </c>
       <c r="L62" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M62" s="5" t="n">
         <v>0</v>
@@ -17656,16 +17656,16 @@
         <v>0</v>
       </c>
       <c r="O62" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P62" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q62" s="4" t="n">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="R62" s="4" t="n">
-        <v>196.67</v>
+        <v>313.33</v>
       </c>
       <c r="S62" s="5" t="n">
         <v>30</v>
@@ -17677,12 +17677,12 @@
       </c>
       <c r="U62" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 15.4€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V62" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 12/01/2025</t>
         </is>
       </c>
       <c r="W62" s="4" t="inlineStr">
@@ -17694,12 +17694,12 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>2707130082</t>
+          <t>2707110022</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
         <is>
-          <t>RASBORA VERDE NEON</t>
+          <t>CORYDORA ORANGE VENEZUELA</t>
         </is>
       </c>
       <c r="C63" s="3" t="inlineStr"/>
@@ -17730,7 +17730,7 @@
         <v>0</v>
       </c>
       <c r="L63" s="4" t="n">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="M63" s="5" t="n">
         <v>0</v>
@@ -17739,7 +17739,7 @@
         <v>0</v>
       </c>
       <c r="O63" s="4" t="n">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="P63" s="4" t="n">
         <v>59</v>
@@ -17760,7 +17760,7 @@
       </c>
       <c r="U63" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 43.13€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 9.58€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V63" s="4" t="inlineStr">
@@ -17777,12 +17777,12 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>2707130041</t>
+          <t>2707120007</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
         <is>
-          <t>POPONDETA FURCATA</t>
+          <t>PANAQUE REAL L190</t>
         </is>
       </c>
       <c r="C64" s="3" t="inlineStr"/>
@@ -17813,7 +17813,7 @@
         <v>0</v>
       </c>
       <c r="L64" s="4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M64" s="5" t="n">
         <v>0</v>
@@ -17822,7 +17822,7 @@
         <v>0</v>
       </c>
       <c r="O64" s="4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="P64" s="4" t="n">
         <v>59</v>
@@ -17843,7 +17843,7 @@
       </c>
       <c r="U64" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 7.31€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 10.72€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V64" s="4" t="inlineStr">
@@ -17860,12 +17860,12 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>2707090010</t>
+          <t>2707040007</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
         <is>
-          <t>KANDANGO ROJO</t>
+          <t>BARBO SAWBWA</t>
         </is>
       </c>
       <c r="C65" s="3" t="inlineStr"/>
@@ -17896,7 +17896,7 @@
         <v>0</v>
       </c>
       <c r="L65" s="4" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="M65" s="5" t="n">
         <v>0</v>
@@ -17905,19 +17905,19 @@
         <v>0</v>
       </c>
       <c r="O65" s="4" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="P65" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q65" s="4" t="n">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="R65" s="4" t="n">
-        <v>393.33</v>
+        <v>33.33</v>
       </c>
       <c r="S65" s="5" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="T65" s="7" t="inlineStr">
         <is>
@@ -17926,12 +17926,12 @@
       </c>
       <c r="U65" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 6.29€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V65" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 23/02/2025</t>
         </is>
       </c>
       <c r="W65" s="4" t="inlineStr">
@@ -17943,32 +17943,24 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>2806030001</t>
+          <t>2707130041</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
         <is>
-          <t>COMETA SURTIDO XXL</t>
-        </is>
-      </c>
-      <c r="C66" s="3" t="inlineStr">
-        <is>
-          <t>15CM</t>
-        </is>
-      </c>
-      <c r="D66" s="3" t="inlineStr">
-        <is>
-          <t>UNICO</t>
-        </is>
-      </c>
+          <t>POPONDETA FURCATA</t>
+        </is>
+      </c>
+      <c r="C66" s="3" t="inlineStr"/>
+      <c r="D66" s="3" t="inlineStr"/>
       <c r="E66" s="4" t="inlineStr">
         <is>
-          <t>2806</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F66" s="4" t="inlineStr">
         <is>
-          <t>PECES JARDIN ACUATICO</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G66" s="4" t="n">
@@ -17987,7 +17979,7 @@
         <v>0</v>
       </c>
       <c r="L66" s="4" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="M66" s="5" t="n">
         <v>0</v>
@@ -17996,7 +17988,7 @@
         <v>0</v>
       </c>
       <c r="O66" s="4" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="P66" s="4" t="n">
         <v>59</v>
@@ -18017,7 +18009,7 @@
       </c>
       <c r="U66" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 14.22€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 7.31€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V66" s="4" t="inlineStr">
@@ -18034,24 +18026,32 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>2707120009</t>
+          <t>2806030001</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
         <is>
-          <t>LORICARIA FILAMENTOSA</t>
-        </is>
-      </c>
-      <c r="C67" s="3" t="inlineStr"/>
-      <c r="D67" s="3" t="inlineStr"/>
+          <t>COMETA SURTIDO XXL</t>
+        </is>
+      </c>
+      <c r="C67" s="3" t="inlineStr">
+        <is>
+          <t>15CM</t>
+        </is>
+      </c>
+      <c r="D67" s="3" t="inlineStr">
+        <is>
+          <t>UNICO</t>
+        </is>
+      </c>
       <c r="E67" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2806</t>
         </is>
       </c>
       <c r="F67" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>PECES JARDIN ACUATICO</t>
         </is>
       </c>
       <c r="G67" s="4" t="n">
@@ -18070,7 +18070,7 @@
         <v>0</v>
       </c>
       <c r="L67" s="4" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M67" s="5" t="n">
         <v>0</v>
@@ -18079,7 +18079,7 @@
         <v>0</v>
       </c>
       <c r="O67" s="4" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="P67" s="4" t="n">
         <v>59</v>
@@ -18100,7 +18100,7 @@
       </c>
       <c r="U67" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 19.74€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 14.22€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V67" s="4" t="inlineStr">
@@ -18117,12 +18117,12 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>2707050028</t>
+          <t>2707110023</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
         <is>
-          <t>BETTA HELLBOY MACHO</t>
+          <t>BOTIA SUMO</t>
         </is>
       </c>
       <c r="C68" s="3" t="inlineStr"/>
@@ -18153,7 +18153,7 @@
         <v>0</v>
       </c>
       <c r="L68" s="4" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M68" s="5" t="n">
         <v>0</v>
@@ -18162,19 +18162,19 @@
         <v>0</v>
       </c>
       <c r="O68" s="4" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="P68" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q68" s="4" t="n">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="R68" s="4" t="n">
-        <v>33.33</v>
+        <v>393.33</v>
       </c>
       <c r="S68" s="5" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="T68" s="7" t="inlineStr">
         <is>
@@ -18183,12 +18183,12 @@
       </c>
       <c r="U68" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 11.13€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V68" s="4" t="inlineStr">
         <is>
-          <t>Compra 23/02/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W68" s="4" t="inlineStr">
@@ -18200,28 +18200,28 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>2204010007</t>
+          <t>2707050021</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
         <is>
-          <t>CONEJO SUPER TOY PEDIGRI (ORYCTOLAGUS CUNICULUS)</t>
+          <t>BESUCON BALON</t>
         </is>
       </c>
       <c r="C69" s="3" t="inlineStr"/>
       <c r="D69" s="3" t="inlineStr"/>
       <c r="E69" s="4" t="inlineStr">
         <is>
-          <t>2204</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F69" s="4" t="inlineStr">
         <is>
-          <t>ANIMAL VIVO PEQUEÑOS MAMIFEROS</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G69" s="4" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H69" s="4" t="n">
         <v>0</v>
@@ -18236,7 +18236,7 @@
         <v>0</v>
       </c>
       <c r="L69" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M69" s="5" t="n">
         <v>0</v>
@@ -18245,16 +18245,16 @@
         <v>0</v>
       </c>
       <c r="O69" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P69" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q69" s="4" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="R69" s="4" t="n">
-        <v>190</v>
+        <v>393.33</v>
       </c>
       <c r="S69" s="5" t="n">
         <v>30</v>
@@ -18266,12 +18266,12 @@
       </c>
       <c r="U69" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 2.04€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V69" s="4" t="inlineStr">
         <is>
-          <t>Compra 02/01/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W69" s="4" t="inlineStr">
@@ -18283,28 +18283,28 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>2707100002</t>
+          <t>2104080001</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
         <is>
-          <t>ANDINOACARA PULCHER AZUL ELECTRICO 3-4</t>
+          <t>PERIQUITO BURQUE</t>
         </is>
       </c>
       <c r="C70" s="3" t="inlineStr"/>
       <c r="D70" s="3" t="inlineStr"/>
       <c r="E70" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2104</t>
         </is>
       </c>
       <c r="F70" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>ANIMAL VIVO PAJARO</t>
         </is>
       </c>
       <c r="G70" s="4" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H70" s="4" t="n">
         <v>0</v>
@@ -18337,7 +18337,7 @@
         <v>59</v>
       </c>
       <c r="R70" s="4" t="n">
-        <v>393.33</v>
+        <v>196.67</v>
       </c>
       <c r="S70" s="5" t="n">
         <v>30</v>
@@ -18349,7 +18349,7 @@
       </c>
       <c r="U70" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 1.47€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 24.5€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V70" s="4" t="inlineStr">
@@ -18366,16 +18366,24 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>2707050021</t>
+          <t>2707110006</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
         <is>
-          <t>BESUCON BALON</t>
-        </is>
-      </c>
-      <c r="C71" s="3" t="inlineStr"/>
-      <c r="D71" s="3" t="inlineStr"/>
+          <t>BOTIA PAYASO</t>
+        </is>
+      </c>
+      <c r="C71" s="3" t="inlineStr">
+        <is>
+          <t>7CM</t>
+        </is>
+      </c>
+      <c r="D71" s="3" t="inlineStr">
+        <is>
+          <t>UNICO</t>
+        </is>
+      </c>
       <c r="E71" s="4" t="inlineStr">
         <is>
           <t>2707</t>
@@ -18432,7 +18440,7 @@
       </c>
       <c r="U71" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 2.04€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 5.91€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V71" s="4" t="inlineStr">
@@ -18449,12 +18457,12 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>2707170002</t>
+          <t>2707130054</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
         <is>
-          <t>PEZ SIERRA SELECTO</t>
+          <t>PEZ CUCHILLO PAYASO</t>
         </is>
       </c>
       <c r="C72" s="3" t="inlineStr"/>
@@ -18485,7 +18493,7 @@
         <v>0</v>
       </c>
       <c r="L72" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M72" s="5" t="n">
         <v>0</v>
@@ -18494,7 +18502,7 @@
         <v>0</v>
       </c>
       <c r="O72" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P72" s="4" t="n">
         <v>59</v>
@@ -18515,7 +18523,7 @@
       </c>
       <c r="U72" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 7.15€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 3.09€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V72" s="4" t="inlineStr">
@@ -18532,24 +18540,16 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>2705040004</t>
+          <t>2705040009</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
         <is>
-          <t>PLANTAS EN TRONCO</t>
-        </is>
-      </c>
-      <c r="C73" s="3" t="inlineStr">
-        <is>
-          <t>3UD</t>
-        </is>
-      </c>
-      <c r="D73" s="3" t="inlineStr">
-        <is>
-          <t>UNICO</t>
-        </is>
-      </c>
+          <t>HELECHO EN COCO PEQUEÑO</t>
+        </is>
+      </c>
+      <c r="C73" s="3" t="inlineStr"/>
+      <c r="D73" s="3" t="inlineStr"/>
       <c r="E73" s="4" t="inlineStr">
         <is>
           <t>2705</t>
@@ -18576,7 +18576,7 @@
         <v>0</v>
       </c>
       <c r="L73" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M73" s="5" t="n">
         <v>0</v>
@@ -18585,7 +18585,7 @@
         <v>0</v>
       </c>
       <c r="O73" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P73" s="4" t="n">
         <v>59</v>
@@ -18606,7 +18606,7 @@
       </c>
       <c r="U73" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 12.35€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 6.52€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V73" s="4" t="inlineStr">
@@ -18623,12 +18623,12 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>2707100040</t>
+          <t>2707130079</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
         <is>
-          <t>RAMIREZI BOLIVIANO (PAPILIOCHROMIS ALTISPINOSA)</t>
+          <t>GOBIO PAVO REAL</t>
         </is>
       </c>
       <c r="C74" s="3" t="inlineStr"/>
@@ -18659,7 +18659,7 @@
         <v>0</v>
       </c>
       <c r="L74" s="4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M74" s="5" t="n">
         <v>0</v>
@@ -18668,16 +18668,16 @@
         <v>0</v>
       </c>
       <c r="O74" s="4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P74" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q74" s="4" t="n">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="R74" s="4" t="n">
-        <v>220</v>
+        <v>393.33</v>
       </c>
       <c r="S74" s="5" t="n">
         <v>30</v>
@@ -18689,12 +18689,12 @@
       </c>
       <c r="U74" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 4.97€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V74" s="4" t="inlineStr">
         <is>
-          <t>Compra 26/01/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W74" s="4" t="inlineStr">
@@ -18706,28 +18706,28 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>2805040003</t>
+          <t>2707130021</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
         <is>
-          <t>PLANTA FLOTANTE MINI</t>
+          <t>MELANOTAENIA SURTIDO</t>
         </is>
       </c>
       <c r="C75" s="3" t="inlineStr"/>
       <c r="D75" s="3" t="inlineStr"/>
       <c r="E75" s="4" t="inlineStr">
         <is>
-          <t>2805</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F75" s="4" t="inlineStr">
         <is>
-          <t>PLANTAS JARDIN ACUATICO</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G75" s="4" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H75" s="4" t="n">
         <v>0</v>
@@ -18742,7 +18742,7 @@
         <v>0</v>
       </c>
       <c r="L75" s="4" t="n">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="M75" s="5" t="n">
         <v>0</v>
@@ -18751,19 +18751,19 @@
         <v>0</v>
       </c>
       <c r="O75" s="4" t="n">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="P75" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q75" s="4" t="n">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="R75" s="4" t="n">
-        <v>173.33</v>
+        <v>126.67</v>
       </c>
       <c r="S75" s="5" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="T75" s="7" t="inlineStr">
         <is>
@@ -18772,12 +18772,12 @@
       </c>
       <c r="U75" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V75" s="4" t="inlineStr">
         <is>
-          <t>Compra 07/01/2025</t>
+          <t>Compra 09/02/2025</t>
         </is>
       </c>
       <c r="W75" s="4" t="inlineStr">
@@ -18789,28 +18789,28 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>2707090002</t>
+          <t>2606050000</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
         <is>
-          <t>CICLIDO TANGANICA SURTIDO</t>
+          <t>BICHO PALO</t>
         </is>
       </c>
       <c r="C76" s="3" t="inlineStr"/>
       <c r="D76" s="3" t="inlineStr"/>
       <c r="E76" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2606</t>
         </is>
       </c>
       <c r="F76" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>ANIMAL VIVO REPTILES</t>
         </is>
       </c>
       <c r="G76" s="4" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H76" s="4" t="n">
         <v>0</v>
@@ -18825,7 +18825,7 @@
         <v>0</v>
       </c>
       <c r="L76" s="4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M76" s="5" t="n">
         <v>0</v>
@@ -18834,19 +18834,19 @@
         <v>0</v>
       </c>
       <c r="O76" s="4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P76" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q76" s="4" t="n">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="R76" s="4" t="n">
-        <v>393.33</v>
+        <v>63.33</v>
       </c>
       <c r="S76" s="5" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="T76" s="7" t="inlineStr">
         <is>
@@ -18855,12 +18855,12 @@
       </c>
       <c r="U76" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 4.9€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V76" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 09/02/2025</t>
         </is>
       </c>
       <c r="W76" s="4" t="inlineStr">
@@ -18872,12 +18872,12 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>2707130079</t>
+          <t>2707050022</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
         <is>
-          <t>GOBIO PAVO REAL</t>
+          <t>BETTA KOI</t>
         </is>
       </c>
       <c r="C77" s="3" t="inlineStr"/>
@@ -18908,7 +18908,7 @@
         <v>0</v>
       </c>
       <c r="L77" s="4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M77" s="5" t="n">
         <v>0</v>
@@ -18917,19 +18917,19 @@
         <v>0</v>
       </c>
       <c r="O77" s="4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P77" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q77" s="4" t="n">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="R77" s="4" t="n">
-        <v>393.33</v>
+        <v>126.67</v>
       </c>
       <c r="S77" s="5" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="T77" s="7" t="inlineStr">
         <is>
@@ -18938,12 +18938,12 @@
       </c>
       <c r="U77" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 4.97€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V77" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 09/02/2025</t>
         </is>
       </c>
       <c r="W77" s="4" t="inlineStr">

</xml_diff>